<commit_message>
Color columns of workbooks for easier understanding
White cells -> Can be used by the user
Gray cells -> Used by Orchestrator Manager
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Assets.xlsx
+++ b/Workbooks/EN/Assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D81BC7F-EFF0-4F3B-8E5E-8DB46372B077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0385109-8009-4715-92CC-658235D16262}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,12 +86,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -116,17 +128,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="27">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -146,9 +169,31 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -157,9 +202,9 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -190,9 +235,9 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -201,20 +246,9 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -229,6 +263,88 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -294,55 +410,8 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -369,17 +438,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:F101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:F101" headerRowDxfId="18" dataDxfId="11">
   <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Organization Unit ID" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Organization Unit Name" totalsRowFunction="count" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="Asset ID"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Asset Name" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
-    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Value" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Organization Unit ID" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Organization Unit Name" totalsRowFunction="count" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="Asset ID" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Asset Name" totalsRowLabel="Total" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Value" dataDxfId="12"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -387,14 +456,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F102" totalsRowShown="0">
   <autoFilter ref="A1:F102" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Organization Unit Name" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Organization Unit Name" dataDxfId="10"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Asset Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value"/>
-    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Asset ID" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Asset ID" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="8"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -402,14 +471,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AFA36666-423E-4267-B808-DBFD2255CE69}" name="Table16" displayName="Table16" ref="A1:F102" totalsRowShown="0">
   <autoFilter ref="A1:F102" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="7" xr3:uid="{45AEE497-3A06-46BE-9F75-8739763D4D01}" name="Organization Unit Name" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{45AEE497-3A06-46BE-9F75-8739763D4D01}" name="Organization Unit Name" dataDxfId="7"/>
     <tableColumn id="1" xr3:uid="{9A783E95-B160-494B-86CA-9B17E7B7BA4E}" name="Asset Name"/>
-    <tableColumn id="3" xr3:uid="{003CF074-AEF0-4160-B2A0-AA78FDEF0550}" name="Username" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{003CF074-AEF0-4160-B2A0-AA78FDEF0550}" name="Username" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{B1103FA1-C444-4B4C-B2DE-2AF1F43EE2F7}" name="Password"/>
-    <tableColumn id="6" xr3:uid="{969717FC-5790-4B75-A1B0-2997BE43FE33}" name="Asset ID" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{6C3F9F68-0351-4140-9C48-3AD60D9434AF}" name="Result" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{969717FC-5790-4B75-A1B0-2997BE43FE33}" name="Asset ID" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{6C3F9F68-0351-4140-9C48-3AD60D9434AF}" name="Result" dataDxfId="4"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -417,13 +486,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD40330C-E043-47F5-9A1D-98C4F5DCAE20}" name="Table15" displayName="Table15" ref="A1:E101" totalsRowShown="0">
   <autoFilter ref="A1:E101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Organization Unit Name" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Asset ID" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Organization Unit Name" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Asset ID" dataDxfId="25"/>
     <tableColumn id="1" xr3:uid="{D002318D-F09E-4941-86F7-CB540B53CA38}" name="Asset Name"/>
     <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="Value"/>
-    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="3"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -431,14 +500,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{343143A2-A745-4DDD-B0DF-0DE2B324A492}" name="Table157" displayName="Table157" ref="A1:F101" totalsRowShown="0">
   <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="7" xr3:uid="{B324D0A3-E152-4308-B124-7203B73A1BBD}" name="Organization Unit Name" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{2934B7C6-CBD1-40B0-AAC0-BB8AE8E4AE77}" name="Asset ID" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{B324D0A3-E152-4308-B124-7203B73A1BBD}" name="Organization Unit Name" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{2934B7C6-CBD1-40B0-AAC0-BB8AE8E4AE77}" name="Asset ID" dataDxfId="23"/>
     <tableColumn id="1" xr3:uid="{672D4252-ECDD-4E80-B35E-6A3063360C37}" name="Asset Name"/>
-    <tableColumn id="2" xr3:uid="{4D4E5EE5-4B2B-487A-B22A-AB3842F3C4E6}" name="Username" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{4D4E5EE5-4B2B-487A-B22A-AB3842F3C4E6}" name="Username" dataDxfId="22"/>
     <tableColumn id="4" xr3:uid="{C7C983FA-5C35-471C-8158-BCB2BC1DC74B}" name="Password"/>
-    <tableColumn id="5" xr3:uid="{67DE61C4-5FA9-48B6-AC2A-1392897C0EF9}" name="Result" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{67DE61C4-5FA9-48B6-AC2A-1392897C0EF9}" name="Result" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -446,13 +515,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:E101" totalsRowShown="0">
   <autoFilter ref="A1:E101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{F24CA0C2-24D3-45F7-8C50-E3B9F93102BC}" name="Organization Unit ID" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Organization Unit Name" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{F81D79E9-4E70-40F0-99EC-DB07CB8A2FD8}" name="Asset ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{F24CA0C2-24D3-45F7-8C50-E3B9F93102BC}" name="Organization Unit ID" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Organization Unit Name" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{F81D79E9-4E70-40F0-99EC-DB07CB8A2FD8}" name="Asset ID" dataDxfId="19"/>
     <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Asset Name" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -736,524 +805,824 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="3"/>
-      <c r="F15" s="1"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
-      <c r="F16" s="1"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="3"/>
-      <c r="F17" s="1"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3"/>
-      <c r="F18" s="1"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="3"/>
-      <c r="F19" s="1"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="3"/>
-      <c r="F20" s="1"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="3"/>
-      <c r="F21" s="1"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="3"/>
-      <c r="F22" s="1"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="3"/>
-      <c r="F23" s="1"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="3"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-      <c r="B25" s="3"/>
-      <c r="F25" s="1"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="3"/>
-      <c r="F26" s="1"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="3"/>
-      <c r="F27" s="1"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="3"/>
-      <c r="F28" s="1"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="3"/>
-      <c r="F29" s="1"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="3"/>
-      <c r="F30" s="1"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
-      <c r="B31" s="3"/>
-      <c r="F31" s="1"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
-      <c r="B32" s="3"/>
-      <c r="F32" s="1"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
-      <c r="B33" s="3"/>
-      <c r="F33" s="1"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
-      <c r="B34" s="3"/>
-      <c r="F34" s="1"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-      <c r="B35" s="3"/>
-      <c r="F35" s="1"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
-      <c r="B36" s="3"/>
-      <c r="F36" s="1"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="1"/>
-      <c r="B37" s="3"/>
-      <c r="F37" s="1"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
-      <c r="B38" s="3"/>
-      <c r="F38" s="1"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
-      <c r="B39" s="3"/>
-      <c r="F39" s="1"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="1"/>
-      <c r="B40" s="3"/>
-      <c r="F40" s="1"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
-      <c r="B41" s="3"/>
-      <c r="F41" s="1"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="1"/>
-      <c r="B42" s="3"/>
-      <c r="F42" s="1"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="1"/>
-      <c r="B43" s="3"/>
-      <c r="F43" s="1"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="1"/>
-      <c r="B44" s="3"/>
-      <c r="F44" s="1"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="1"/>
-      <c r="B45" s="3"/>
-      <c r="F45" s="1"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="1"/>
-      <c r="B46" s="3"/>
-      <c r="F46" s="1"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="1"/>
-      <c r="B47" s="3"/>
-      <c r="F47" s="1"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="1"/>
-      <c r="B48" s="3"/>
-      <c r="F48" s="1"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="1"/>
-      <c r="B49" s="3"/>
-      <c r="F49" s="1"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="1"/>
-      <c r="B50" s="3"/>
-      <c r="F50" s="1"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="1"/>
-      <c r="B51" s="3"/>
-      <c r="F51" s="1"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="1"/>
-      <c r="B52" s="3"/>
-      <c r="F52" s="1"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="1"/>
-      <c r="B53" s="3"/>
-      <c r="F53" s="1"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="1"/>
-      <c r="B54" s="3"/>
-      <c r="F54" s="1"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="1"/>
-      <c r="B55" s="3"/>
-      <c r="F55" s="1"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="1"/>
-      <c r="B56" s="3"/>
-      <c r="F56" s="1"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="1"/>
-      <c r="B57" s="3"/>
-      <c r="F57" s="1"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="1"/>
-      <c r="B58" s="3"/>
-      <c r="F58" s="1"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="1"/>
-      <c r="B59" s="3"/>
-      <c r="F59" s="1"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="1"/>
-      <c r="B60" s="3"/>
-      <c r="F60" s="1"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="1"/>
-      <c r="B61" s="3"/>
-      <c r="F61" s="1"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="1"/>
-      <c r="B62" s="3"/>
-      <c r="F62" s="1"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="1"/>
-      <c r="B63" s="3"/>
-      <c r="F63" s="1"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="1"/>
-      <c r="B64" s="3"/>
-      <c r="F64" s="1"/>
+      <c r="A64" s="9"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" s="1"/>
-      <c r="B65" s="3"/>
-      <c r="F65" s="1"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="1"/>
-      <c r="B66" s="3"/>
-      <c r="F66" s="1"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="1"/>
-      <c r="B67" s="3"/>
-      <c r="F67" s="1"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="1"/>
-      <c r="B68" s="3"/>
-      <c r="F68" s="1"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="1"/>
-      <c r="B69" s="3"/>
-      <c r="F69" s="1"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="1"/>
-      <c r="B70" s="3"/>
-      <c r="F70" s="1"/>
+      <c r="A70" s="9"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="1"/>
-      <c r="B71" s="3"/>
-      <c r="F71" s="1"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="1"/>
-      <c r="B72" s="3"/>
-      <c r="F72" s="1"/>
+      <c r="A72" s="9"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="1"/>
-      <c r="B73" s="3"/>
-      <c r="F73" s="1"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="1"/>
-      <c r="B74" s="3"/>
-      <c r="F74" s="1"/>
+      <c r="A74" s="9"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="1"/>
-      <c r="B75" s="3"/>
-      <c r="F75" s="1"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="1"/>
-      <c r="B76" s="3"/>
-      <c r="F76" s="1"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="1"/>
-      <c r="B77" s="3"/>
-      <c r="F77" s="1"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="1"/>
-      <c r="B78" s="3"/>
-      <c r="F78" s="1"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A79" s="1"/>
-      <c r="B79" s="3"/>
-      <c r="F79" s="1"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A80" s="1"/>
-      <c r="B80" s="3"/>
-      <c r="F80" s="1"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81" s="1"/>
-      <c r="B81" s="3"/>
-      <c r="F81" s="1"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" s="1"/>
-      <c r="B82" s="3"/>
-      <c r="F82" s="1"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A83" s="1"/>
-      <c r="B83" s="3"/>
-      <c r="F83" s="1"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84" s="1"/>
-      <c r="B84" s="3"/>
-      <c r="F84" s="1"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" s="1"/>
-      <c r="B85" s="3"/>
-      <c r="F85" s="1"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="1"/>
-      <c r="B86" s="3"/>
-      <c r="F86" s="1"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="10"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" s="1"/>
-      <c r="B87" s="3"/>
-      <c r="F87" s="1"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="10"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88" s="1"/>
-      <c r="B88" s="3"/>
-      <c r="F88" s="1"/>
+      <c r="A88" s="9"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89" s="1"/>
-      <c r="B89" s="3"/>
-      <c r="F89" s="1"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90" s="1"/>
-      <c r="B90" s="3"/>
-      <c r="F90" s="1"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A91" s="1"/>
-      <c r="B91" s="3"/>
-      <c r="F91" s="1"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" s="1"/>
-      <c r="B92" s="3"/>
-      <c r="F92" s="1"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A93" s="1"/>
-      <c r="B93" s="3"/>
-      <c r="F93" s="1"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A94" s="1"/>
-      <c r="B94" s="3"/>
-      <c r="F94" s="1"/>
+      <c r="A94" s="9"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A95" s="1"/>
-      <c r="B95" s="3"/>
-      <c r="F95" s="1"/>
+      <c r="A95" s="9"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A96" s="1"/>
-      <c r="B96" s="3"/>
-      <c r="F96" s="1"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A97" s="1"/>
-      <c r="B97" s="3"/>
-      <c r="F97" s="1"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="10"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A98" s="1"/>
-      <c r="B98" s="3"/>
-      <c r="F98" s="1"/>
+      <c r="A98" s="9"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A99" s="1"/>
-      <c r="B99" s="3"/>
-      <c r="F99" s="1"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="10"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A100" s="1"/>
-      <c r="B100" s="3"/>
-      <c r="F100" s="1"/>
+      <c r="A100" s="9"/>
+      <c r="B100" s="10"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A101" s="1"/>
-      <c r="B101" s="3"/>
-      <c r="F101" s="1"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="10"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1300,618 +1669,618 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="1"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="D59" s="2"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
       <c r="D61" s="2"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="D69" s="2"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="D71" s="2"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="D73" s="2"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="D75" s="2"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
       <c r="D79" s="2"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
       <c r="D80" s="2"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="D81" s="2"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="D82" s="2"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="D83" s="2"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="D84" s="2"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="D85" s="2"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="D86" s="2"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="D87" s="2"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="D88" s="2"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="D91" s="2"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="D92" s="2"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="D93" s="2"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="D98" s="2"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="D99" s="2"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="D100" s="2"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="D101" s="2"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
       <c r="D102" s="2"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1959,426 +2328,618 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="D5" s="4"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="D13" s="4"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="D14" s="4"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="D15" s="4"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
       <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
       <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
       <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
       <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
       <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
       <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="4"/>
       <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="4"/>
       <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="4"/>
       <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="4"/>
       <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="4"/>
       <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="4"/>
       <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
       <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="4"/>
       <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="4"/>
       <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="4"/>
       <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
       <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="4"/>
       <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="4"/>
       <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="4"/>
       <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
       <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="4"/>
       <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
       <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="4"/>
       <c r="D59" s="4"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="4"/>
       <c r="D60" s="4"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
       <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
       <c r="D62" s="4"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
       <c r="D63" s="4"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
       <c r="D64" s="4"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="4"/>
       <c r="D65" s="4"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="4"/>
       <c r="D66" s="4"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="4"/>
       <c r="D67" s="4"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="4"/>
       <c r="D68" s="4"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="4"/>
       <c r="D69" s="4"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="4"/>
       <c r="D70" s="4"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="4"/>
       <c r="D71" s="4"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="4"/>
       <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="4"/>
       <c r="D73" s="4"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="4"/>
       <c r="D74" s="4"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="4"/>
       <c r="D75" s="4"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="4"/>
       <c r="D76" s="4"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="4"/>
       <c r="D77" s="4"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="4"/>
       <c r="D78" s="4"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="4"/>
       <c r="D79" s="4"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="4"/>
       <c r="D80" s="4"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="4"/>
       <c r="D81" s="4"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="4"/>
       <c r="D82" s="4"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="4"/>
       <c r="D83" s="4"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="4"/>
       <c r="D84" s="4"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="4"/>
       <c r="D85" s="4"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="4"/>
       <c r="D86" s="4"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="4"/>
       <c r="D87" s="4"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="4"/>
       <c r="D88" s="4"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="4"/>
       <c r="D89" s="4"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="4"/>
       <c r="D90" s="4"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="4"/>
       <c r="D91" s="4"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="4"/>
       <c r="D92" s="4"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="4"/>
       <c r="D93" s="4"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="4"/>
       <c r="D94" s="4"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="4"/>
       <c r="D95" s="4"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="4"/>
       <c r="D96" s="4"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E96" s="8"/>
+      <c r="F96" s="8"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="4"/>
       <c r="D97" s="4"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E97" s="8"/>
+      <c r="F97" s="8"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="4"/>
       <c r="D98" s="4"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E98" s="8"/>
+      <c r="F98" s="8"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="4"/>
       <c r="D99" s="4"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="4"/>
       <c r="D100" s="4"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="4"/>
       <c r="D101" s="4"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="4"/>
       <c r="D102" s="4"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2419,509 +2980,509 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="E24" s="2"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="E29" s="2"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="E30" s="2"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="E31" s="2"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="E34" s="2"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="E35" s="2"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="E36" s="2"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="E37" s="2"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="E38" s="2"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="E39" s="2"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="E40" s="2"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="E41" s="2"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="E42" s="2"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="E43" s="2"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="E44" s="2"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="E45" s="2"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="E46" s="2"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="E47" s="2"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="E48" s="2"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="E49" s="2"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="E50" s="2"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="E51" s="2"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="E52" s="2"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="E53" s="2"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="E54" s="2"/>
+      <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="E55" s="2"/>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="E56" s="2"/>
+      <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="E57" s="2"/>
+      <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="E58" s="2"/>
+      <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="E59" s="2"/>
+      <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="E60" s="2"/>
+      <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="E61" s="2"/>
+      <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="E62" s="2"/>
+      <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="E63" s="2"/>
+      <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="E64" s="2"/>
+      <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="E65" s="2"/>
+      <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
-      <c r="E66" s="2"/>
+      <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
-      <c r="E67" s="2"/>
+      <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="E68" s="2"/>
+      <c r="E68" s="7"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="E69" s="2"/>
+      <c r="E69" s="7"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-      <c r="E70" s="2"/>
+      <c r="E70" s="7"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-      <c r="E71" s="2"/>
+      <c r="E71" s="7"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
-      <c r="E72" s="2"/>
+      <c r="E72" s="7"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="E73" s="2"/>
+      <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="E74" s="2"/>
+      <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="E75" s="2"/>
+      <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
-      <c r="E76" s="2"/>
+      <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="E77" s="2"/>
+      <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="E78" s="2"/>
+      <c r="E78" s="7"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="E79" s="2"/>
+      <c r="E79" s="7"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="E80" s="2"/>
+      <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="E81" s="2"/>
+      <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-      <c r="E82" s="2"/>
+      <c r="E82" s="7"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
-      <c r="E83" s="2"/>
+      <c r="E83" s="7"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-      <c r="E84" s="2"/>
+      <c r="E84" s="7"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
-      <c r="E85" s="2"/>
+      <c r="E85" s="7"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
-      <c r="E86" s="2"/>
+      <c r="E86" s="7"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
-      <c r="E87" s="2"/>
+      <c r="E87" s="7"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
-      <c r="E88" s="2"/>
+      <c r="E88" s="7"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
-      <c r="E89" s="2"/>
+      <c r="E89" s="7"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
-      <c r="E90" s="2"/>
+      <c r="E90" s="7"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
-      <c r="E91" s="2"/>
+      <c r="E91" s="7"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="E92" s="2"/>
+      <c r="E92" s="7"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
-      <c r="E93" s="2"/>
+      <c r="E93" s="7"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-      <c r="E94" s="2"/>
+      <c r="E94" s="7"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
-      <c r="E95" s="2"/>
+      <c r="E95" s="7"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
-      <c r="E96" s="2"/>
+      <c r="E96" s="7"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
-      <c r="E97" s="2"/>
+      <c r="E97" s="7"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
-      <c r="E98" s="2"/>
+      <c r="E98" s="7"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
-      <c r="E99" s="2"/>
+      <c r="E99" s="7"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
-      <c r="E100" s="2"/>
+      <c r="E100" s="7"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
-      <c r="E101" s="2"/>
+      <c r="E101" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2967,421 +3528,421 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B18"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B19"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B20"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B21"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B22"/>
-      <c r="F22" s="4"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B23"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B24"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B25"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B26"/>
-      <c r="F26" s="4"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B29"/>
-      <c r="F29" s="4"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30"/>
-      <c r="F30" s="4"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31"/>
-      <c r="F31" s="4"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32"/>
-      <c r="F32" s="4"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33"/>
-      <c r="F33" s="4"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34"/>
-      <c r="F34" s="4"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35"/>
-      <c r="F35" s="4"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36"/>
-      <c r="F36" s="4"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B37"/>
-      <c r="F37" s="4"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38"/>
-      <c r="F38" s="4"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39"/>
-      <c r="F39" s="4"/>
+      <c r="F39" s="11"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B40"/>
-      <c r="F40" s="4"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B41"/>
-      <c r="F41" s="4"/>
+      <c r="F41" s="11"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B42"/>
-      <c r="F42" s="4"/>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43"/>
-      <c r="F43" s="4"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B44"/>
-      <c r="F44" s="4"/>
+      <c r="F44" s="11"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B45"/>
-      <c r="F45" s="4"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B46"/>
-      <c r="F46" s="4"/>
+      <c r="F46" s="11"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B47"/>
-      <c r="F47" s="4"/>
+      <c r="F47" s="11"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B48"/>
-      <c r="F48" s="4"/>
+      <c r="F48" s="11"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B49"/>
-      <c r="F49" s="4"/>
+      <c r="F49" s="11"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B50"/>
-      <c r="F50" s="4"/>
+      <c r="F50" s="11"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B51"/>
-      <c r="F51" s="4"/>
+      <c r="F51" s="11"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B52"/>
-      <c r="F52" s="4"/>
+      <c r="F52" s="11"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B53"/>
-      <c r="F53" s="4"/>
+      <c r="F53" s="11"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B54"/>
-      <c r="F54" s="4"/>
+      <c r="F54" s="11"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B55"/>
-      <c r="F55" s="4"/>
+      <c r="F55" s="11"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B56"/>
-      <c r="F56" s="4"/>
+      <c r="F56" s="11"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B57"/>
-      <c r="F57" s="4"/>
+      <c r="F57" s="11"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B58"/>
-      <c r="F58" s="4"/>
+      <c r="F58" s="11"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B59"/>
-      <c r="F59" s="4"/>
+      <c r="F59" s="11"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B60"/>
-      <c r="F60" s="4"/>
+      <c r="F60" s="11"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B61"/>
-      <c r="F61" s="4"/>
+      <c r="F61" s="11"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B62"/>
-      <c r="F62" s="4"/>
+      <c r="F62" s="11"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B63"/>
-      <c r="F63" s="4"/>
+      <c r="F63" s="11"/>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B64"/>
-      <c r="F64" s="4"/>
+      <c r="F64" s="11"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B65"/>
-      <c r="F65" s="4"/>
+      <c r="F65" s="11"/>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B66"/>
-      <c r="F66" s="4"/>
+      <c r="F66" s="11"/>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B67"/>
-      <c r="F67" s="4"/>
+      <c r="F67" s="11"/>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B68"/>
-      <c r="F68" s="4"/>
+      <c r="F68" s="11"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B69"/>
-      <c r="F69" s="4"/>
+      <c r="F69" s="11"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B70"/>
-      <c r="F70" s="4"/>
+      <c r="F70" s="11"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B71"/>
-      <c r="F71" s="4"/>
+      <c r="F71" s="11"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B72"/>
-      <c r="F72" s="4"/>
+      <c r="F72" s="11"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B73"/>
-      <c r="F73" s="4"/>
+      <c r="F73" s="11"/>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B74"/>
-      <c r="F74" s="4"/>
+      <c r="F74" s="11"/>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B75"/>
-      <c r="F75" s="4"/>
+      <c r="F75" s="11"/>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B76"/>
-      <c r="F76" s="4"/>
+      <c r="F76" s="11"/>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B77"/>
-      <c r="F77" s="4"/>
+      <c r="F77" s="11"/>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B78"/>
-      <c r="F78" s="4"/>
+      <c r="F78" s="11"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B79"/>
-      <c r="F79" s="4"/>
+      <c r="F79" s="11"/>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B80"/>
-      <c r="F80" s="4"/>
+      <c r="F80" s="11"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B81"/>
-      <c r="F81" s="4"/>
+      <c r="F81" s="11"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B82"/>
-      <c r="F82" s="4"/>
+      <c r="F82" s="11"/>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B83"/>
-      <c r="F83" s="4"/>
+      <c r="F83" s="11"/>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B84"/>
-      <c r="F84" s="4"/>
+      <c r="F84" s="11"/>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B85"/>
-      <c r="F85" s="4"/>
+      <c r="F85" s="11"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B86"/>
-      <c r="F86" s="4"/>
+      <c r="F86" s="11"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B87"/>
-      <c r="F87" s="4"/>
+      <c r="F87" s="11"/>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B88"/>
-      <c r="F88" s="4"/>
+      <c r="F88" s="11"/>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B89"/>
-      <c r="F89" s="4"/>
+      <c r="F89" s="11"/>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B90"/>
-      <c r="F90" s="4"/>
+      <c r="F90" s="11"/>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B91"/>
-      <c r="F91" s="4"/>
+      <c r="F91" s="11"/>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B92"/>
-      <c r="F92" s="4"/>
+      <c r="F92" s="11"/>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B93"/>
-      <c r="F93" s="4"/>
+      <c r="F93" s="11"/>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B94"/>
-      <c r="F94" s="4"/>
+      <c r="F94" s="11"/>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B95"/>
-      <c r="F95" s="4"/>
+      <c r="F95" s="11"/>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B96"/>
-      <c r="F96" s="4"/>
+      <c r="F96" s="11"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B97"/>
-      <c r="F97" s="4"/>
+      <c r="F97" s="11"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B98"/>
-      <c r="F98" s="4"/>
+      <c r="F98" s="11"/>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B99"/>
-      <c r="F99" s="4"/>
+      <c r="F99" s="11"/>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B100"/>
-      <c r="F100" s="4"/>
+      <c r="F100" s="11"/>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B101"/>
-      <c r="F101" s="4"/>
+      <c r="F101" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3422,7 +3983,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3430,502 +3991,503 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="D6" s="1"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="1"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="1"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="1"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="1"/>
+      <c r="E36" s="9"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="1"/>
+      <c r="E37" s="9"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="1"/>
+      <c r="E38" s="9"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="1"/>
+      <c r="E39" s="9"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="1"/>
+      <c r="E40" s="9"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="1"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="1"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="1"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="1"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="1"/>
+      <c r="E45" s="9"/>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="1"/>
+      <c r="E46" s="9"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="1"/>
+      <c r="E47" s="9"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="1"/>
+      <c r="E48" s="9"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="1"/>
+      <c r="E49" s="9"/>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C50" s="1"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="1"/>
+      <c r="E50" s="9"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C51" s="1"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="1"/>
+      <c r="E51" s="9"/>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C52" s="1"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="1"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C53" s="1"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="1"/>
+      <c r="E53" s="9"/>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C54" s="1"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="1"/>
+      <c r="E54" s="9"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C55" s="1"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="1"/>
+      <c r="E55" s="9"/>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C56" s="1"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="1"/>
+      <c r="E56" s="9"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C57" s="1"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="1"/>
+      <c r="E57" s="9"/>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C58" s="1"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="1"/>
+      <c r="E58" s="9"/>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C59" s="1"/>
       <c r="D59" s="2"/>
-      <c r="E59" s="1"/>
+      <c r="E59" s="9"/>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C60" s="1"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="1"/>
+      <c r="E60" s="9"/>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C61" s="1"/>
       <c r="D61" s="2"/>
-      <c r="E61" s="1"/>
+      <c r="E61" s="9"/>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C62" s="1"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="1"/>
+      <c r="E62" s="9"/>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C63" s="1"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="1"/>
+      <c r="E63" s="9"/>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C64" s="1"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="1"/>
+      <c r="E64" s="9"/>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C65" s="1"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="1"/>
+      <c r="E65" s="9"/>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C66" s="1"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="1"/>
+      <c r="E66" s="9"/>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C67" s="1"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="1"/>
+      <c r="E67" s="9"/>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C68" s="1"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="1"/>
+      <c r="E68" s="9"/>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C69" s="1"/>
       <c r="D69" s="2"/>
-      <c r="E69" s="1"/>
+      <c r="E69" s="9"/>
     </row>
     <row r="70" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C70" s="1"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="1"/>
+      <c r="E70" s="9"/>
     </row>
     <row r="71" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C71" s="1"/>
       <c r="D71" s="2"/>
-      <c r="E71" s="1"/>
+      <c r="E71" s="9"/>
     </row>
     <row r="72" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="1"/>
+      <c r="E72" s="9"/>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
-      <c r="E73" s="1"/>
+      <c r="E73" s="9"/>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C74" s="1"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="1"/>
+      <c r="E74" s="9"/>
     </row>
     <row r="75" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
-      <c r="E75" s="1"/>
+      <c r="E75" s="9"/>
     </row>
     <row r="76" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C76" s="1"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="1"/>
+      <c r="E76" s="9"/>
     </row>
     <row r="77" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C77" s="1"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="1"/>
+      <c r="E77" s="9"/>
     </row>
     <row r="78" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C78" s="1"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="1"/>
+      <c r="E78" s="9"/>
     </row>
     <row r="79" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
+      <c r="E79" s="9"/>
     </row>
     <row r="80" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
+      <c r="E80" s="9"/>
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
+      <c r="E81" s="9"/>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
+      <c r="E82" s="9"/>
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
+      <c r="E83" s="9"/>
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
+      <c r="E84" s="9"/>
     </row>
     <row r="85" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
+      <c r="E85" s="9"/>
     </row>
     <row r="86" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
+      <c r="E86" s="9"/>
     </row>
     <row r="87" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
+      <c r="E87" s="9"/>
     </row>
     <row r="88" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
+      <c r="E88" s="9"/>
     </row>
     <row r="89" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
+      <c r="E89" s="9"/>
     </row>
     <row r="90" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
+      <c r="E90" s="9"/>
     </row>
     <row r="91" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
+      <c r="E91" s="9"/>
     </row>
     <row r="92" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
+      <c r="E92" s="9"/>
     </row>
     <row r="93" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
+      <c r="E93" s="9"/>
     </row>
     <row r="94" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
+      <c r="E94" s="9"/>
     </row>
     <row r="95" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
+      <c r="E95" s="9"/>
     </row>
     <row r="96" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
+      <c r="E96" s="9"/>
     </row>
     <row r="97" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
+      <c r="E97" s="9"/>
     </row>
     <row r="98" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
+      <c r="E98" s="9"/>
     </row>
     <row r="99" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
+      <c r="E99" s="9"/>
     </row>
     <row r="100" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
+      <c r="E100" s="9"/>
     </row>
     <row r="101" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
+      <c r="E101" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Implement Get Credential Assets operation
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Assets.xlsx
+++ b/Workbooks/EN/Assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38139DB0-466D-436A-ACE5-E2DE7E46A963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5B7587-E925-4C02-9AD1-AADB6E783F45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="15">
   <si>
     <t>Asset ID</t>
   </si>
@@ -402,7 +402,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="58">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1298,56 +1298,6 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1846,34 +1796,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:I201" headerRowDxfId="59" dataDxfId="57" totalsRowDxfId="55" headerRowBorderDxfId="58" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:I201" headerRowDxfId="57" dataDxfId="55" totalsRowDxfId="53" headerRowBorderDxfId="56" tableBorderDxfId="54">
   <autoFilter ref="A1:I201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Folder ID" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Name" totalsRowFunction="count" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="Asset ID" dataDxfId="52"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Asset Name" totalsRowLabel="Total" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{8E6D9239-8D17-4851-B81E-AA3B7A84B18A}" name="Scope" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{57694A87-E20F-4EA5-8070-3065D32AB335}" name="Robot or User ID" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{E62E1B92-1422-4B09-9336-6FC76D703F22}" name="Robot or User Name" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Value" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Folder ID" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Name" totalsRowFunction="count" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="Asset ID" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Asset Name" totalsRowLabel="Total" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{8E6D9239-8D17-4851-B81E-AA3B7A84B18A}" name="Scope" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{57694A87-E20F-4EA5-8070-3065D32AB335}" name="Robot or User ID" dataDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{E62E1B92-1422-4B09-9336-6FC76D703F22}" name="Robot or User Name" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Value" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9BB38C27-A0FF-4D4F-AD77-24125AC0FC70}" name="Table148" displayName="Table148" ref="A1:I201" headerRowDxfId="45" dataDxfId="43" totalsRowDxfId="41" headerRowBorderDxfId="44" tableBorderDxfId="42">
-  <autoFilter ref="A1:I201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="9">
-    <tableColumn id="6" xr3:uid="{485E597C-A24C-40C0-A3EE-E03068634948}" name="Folder ID" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{B6D8F5D0-41CD-4EF8-84D7-03F38C71AB1B}" name="Folder Name" totalsRowFunction="count" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{7208AC74-66FB-4CA6-B9B5-7263FD360340}" name="Credential Asset ID" dataDxfId="38"/>
-    <tableColumn id="1" xr3:uid="{003DAFDE-C24E-41F7-82CA-B0B481F221E2}" name="Credential Asset Name" totalsRowLabel="Total" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{E44775CD-BBCF-4B36-BAE6-DECF89D643E9}" name="Scope" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{BA8C9509-9B8E-4CF6-A2DD-70512D0BB9A6}" name="Robot or User ID" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{C4F99EC1-76A9-472A-A520-E6C2C7DA3F6B}" name="Robot or User Name" dataDxfId="34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9BB38C27-A0FF-4D4F-AD77-24125AC0FC70}" name="Table148" displayName="Table148" ref="A1:G201" headerRowDxfId="43" dataDxfId="41" totalsRowDxfId="39" headerRowBorderDxfId="42" tableBorderDxfId="40">
+  <autoFilter ref="A1:G201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="6" xr3:uid="{485E597C-A24C-40C0-A3EE-E03068634948}" name="Folder ID" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{B6D8F5D0-41CD-4EF8-84D7-03F38C71AB1B}" name="Folder Name" totalsRowFunction="count" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{7208AC74-66FB-4CA6-B9B5-7263FD360340}" name="Credential Asset ID" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{003DAFDE-C24E-41F7-82CA-B0B481F221E2}" name="Credential Asset Name" totalsRowLabel="Total" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{E44775CD-BBCF-4B36-BAE6-DECF89D643E9}" name="Scope" dataDxfId="34"/>
     <tableColumn id="7" xr3:uid="{DF92207D-0652-4129-89C3-EB38552DB3A7}" name="Username" dataDxfId="33"/>
     <tableColumn id="4" xr3:uid="{FBA4015B-2D60-460E-9719-EA2C2B95F766}" name="Password" dataDxfId="32" totalsRowDxfId="31"/>
   </tableColumns>
@@ -4492,7 +4440,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6344F8B8-E12C-4A10-9CFE-BCB8BEC8153F}">
-  <dimension ref="A1:I201"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -4505,10 +4453,10 @@
     <col min="3" max="3" width="25.7109375" style="34" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="9" width="25.7109375" customWidth="1"/>
+    <col min="6" max="7" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -4525,2217 +4473,1811 @@
         <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="G1" s="47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="6"/>
       <c r="C2" s="10"/>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="45"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="8"/>
+      <c r="G2" s="45"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="6"/>
       <c r="C3" s="10"/>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="44"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="8"/>
+      <c r="G3" s="44"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="6"/>
       <c r="C4" s="10"/>
       <c r="D4" s="7"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="44"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="8"/>
+      <c r="G4" s="44"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="6"/>
       <c r="C5" s="10"/>
       <c r="D5" s="7"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="44"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" s="8"/>
+      <c r="G5" s="44"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="6"/>
       <c r="C6" s="10"/>
       <c r="D6" s="7"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="44"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="8"/>
+      <c r="G6" s="44"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="6"/>
       <c r="C7" s="10"/>
       <c r="D7" s="7"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="44"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="8"/>
+      <c r="G7" s="44"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="6"/>
       <c r="C8" s="10"/>
       <c r="D8" s="7"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="44"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F8" s="8"/>
+      <c r="G8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
       <c r="D9" s="7"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="44"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="8"/>
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
       <c r="D10" s="7"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="44"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F10" s="8"/>
+      <c r="G10" s="44"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="32"/>
       <c r="B11" s="7"/>
       <c r="C11" s="10"/>
       <c r="D11" s="7"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="44"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="44"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="32"/>
       <c r="B12" s="7"/>
       <c r="C12" s="10"/>
       <c r="D12" s="7"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="44"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="44"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
       <c r="B13" s="7"/>
       <c r="C13" s="10"/>
       <c r="D13" s="7"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="44"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="44"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
       <c r="B14" s="7"/>
       <c r="C14" s="10"/>
       <c r="D14" s="7"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="44"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="44"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="32"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="7"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="44"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="44"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="32"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="7"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="44"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="44"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="32"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="7"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="44"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G17" s="44"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="32"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="7"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="44"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="44"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="32"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="7"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="44"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19" s="44"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="32"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="7"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="44"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G20" s="44"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="32"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="7"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="44"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G21" s="44"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="32"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="7"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="44"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="44"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="32"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="7"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="44"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G23" s="44"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="32"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="7"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="44"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="44"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="32"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="7"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="44"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="44"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="32"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="7"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="44"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="44"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="32"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="7"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="44"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="44"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="32"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="7"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="44"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="44"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="32"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="7"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="44"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="44"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="32"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="7"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="44"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="44"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="7"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="44"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="44"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="32"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="7"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="44"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G32" s="44"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="7"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="44"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G33" s="44"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="32"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="7"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="44"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G34" s="44"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="32"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="7"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="44"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="44"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="32"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="7"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="44"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G36" s="44"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="32"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="7"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="44"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G37" s="44"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="32"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="7"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="44"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G38" s="44"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="32"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="7"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="44"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G39" s="44"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="32"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="7"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="44"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G40" s="44"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="32"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="7"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="44"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G41" s="44"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="32"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="7"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="44"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G42" s="44"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="32"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="7"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="44"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G43" s="44"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="32"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="7"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="44"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G44" s="44"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="32"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="7"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="44"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G45" s="44"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="32"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="7"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="44"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G46" s="44"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="32"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="7"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="44"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G47" s="44"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="32"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="7"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="44"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G48" s="44"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="32"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="7"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="44"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G49" s="44"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="32"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="7"/>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="44"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G50" s="44"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="32"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="7"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="44"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G51" s="44"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="32"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="7"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="44"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="44"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="32"/>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="7"/>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="44"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="44"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="32"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="7"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="44"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="44"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="32"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="7"/>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="44"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="44"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="32"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="7"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="44"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="44"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="32"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="7"/>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="44"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G57" s="44"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="32"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="7"/>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="44"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G58" s="44"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="32"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="7"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="44"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G59" s="44"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="32"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="7"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="44"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="44"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="32"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="7"/>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="44"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G61" s="44"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="32"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="7"/>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="44"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="44"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="32"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="7"/>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="44"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G63" s="44"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="32"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="7"/>
       <c r="E64" s="9"/>
       <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="44"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G64" s="44"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="32"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="7"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="44"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G65" s="44"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="32"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="7"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="44"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G66" s="44"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="32"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="7"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="44"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G67" s="44"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="32"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="D68" s="7"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="44"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G68" s="44"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="32"/>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="D69" s="7"/>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="44"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G69" s="44"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="32"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="7"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="44"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G70" s="44"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="32"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="7"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="44"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G71" s="44"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="32"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="7"/>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="44"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G72" s="44"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="32"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
       <c r="D73" s="7"/>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="44"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G73" s="44"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="32"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="7"/>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="44"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G74" s="44"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="32"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
       <c r="D75" s="7"/>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="44"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G75" s="44"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="32"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
       <c r="D76" s="7"/>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="44"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G76" s="44"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="32"/>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
       <c r="D77" s="7"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="44"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G77" s="44"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="32"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
       <c r="D78" s="7"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="44"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G78" s="44"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="32"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
       <c r="D79" s="7"/>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="44"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G79" s="44"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="32"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="7"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="44"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G80" s="44"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="32"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="7"/>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="44"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G81" s="44"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="32"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
       <c r="D82" s="7"/>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="44"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G82" s="44"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="32"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
       <c r="D83" s="7"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
-      <c r="G83" s="9"/>
-      <c r="H83" s="9"/>
-      <c r="I83" s="44"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G83" s="44"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="32"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
       <c r="D84" s="7"/>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="44"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G84" s="44"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="32"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
       <c r="D85" s="7"/>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
-      <c r="H85" s="9"/>
-      <c r="I85" s="44"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G85" s="44"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="32"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
       <c r="D86" s="7"/>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
-      <c r="I86" s="44"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G86" s="44"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="32"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
       <c r="D87" s="7"/>
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
-      <c r="G87" s="9"/>
-      <c r="H87" s="9"/>
-      <c r="I87" s="44"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G87" s="44"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="32"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
       <c r="D88" s="7"/>
       <c r="E88" s="9"/>
       <c r="F88" s="9"/>
-      <c r="G88" s="9"/>
-      <c r="H88" s="9"/>
-      <c r="I88" s="44"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G88" s="44"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="32"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
       <c r="D89" s="7"/>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
-      <c r="G89" s="9"/>
-      <c r="H89" s="9"/>
-      <c r="I89" s="44"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G89" s="44"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="32"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
       <c r="D90" s="7"/>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
-      <c r="G90" s="9"/>
-      <c r="H90" s="9"/>
-      <c r="I90" s="44"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G90" s="44"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="32"/>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
       <c r="D91" s="7"/>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
-      <c r="G91" s="9"/>
-      <c r="H91" s="9"/>
-      <c r="I91" s="44"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G91" s="44"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="32"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
       <c r="D92" s="7"/>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
-      <c r="H92" s="9"/>
-      <c r="I92" s="44"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G92" s="44"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="32"/>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
       <c r="D93" s="7"/>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
-      <c r="G93" s="9"/>
-      <c r="H93" s="9"/>
-      <c r="I93" s="44"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G93" s="44"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="32"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
       <c r="D94" s="7"/>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
-      <c r="G94" s="9"/>
-      <c r="H94" s="9"/>
-      <c r="I94" s="44"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G94" s="44"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="32"/>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="7"/>
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
-      <c r="G95" s="9"/>
-      <c r="H95" s="9"/>
-      <c r="I95" s="44"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G95" s="44"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="32"/>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="7"/>
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
-      <c r="G96" s="9"/>
-      <c r="H96" s="9"/>
-      <c r="I96" s="44"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G96" s="44"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="32"/>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
       <c r="D97" s="7"/>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
-      <c r="G97" s="9"/>
-      <c r="H97" s="9"/>
-      <c r="I97" s="44"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G97" s="44"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="32"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="7"/>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
-      <c r="G98" s="9"/>
-      <c r="H98" s="9"/>
-      <c r="I98" s="44"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G98" s="44"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="32"/>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="7"/>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
-      <c r="G99" s="9"/>
-      <c r="H99" s="9"/>
-      <c r="I99" s="44"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G99" s="44"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="32"/>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
       <c r="D100" s="7"/>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
-      <c r="G100" s="9"/>
-      <c r="H100" s="9"/>
-      <c r="I100" s="44"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G100" s="44"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
       <c r="B101" s="11"/>
       <c r="C101" s="11"/>
       <c r="D101" s="12"/>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="44"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G101" s="44"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="32"/>
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
       <c r="D102" s="7"/>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="9"/>
-      <c r="I102" s="44"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G102" s="44"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="32"/>
       <c r="B103" s="10"/>
       <c r="C103" s="10"/>
       <c r="D103" s="7"/>
       <c r="E103" s="9"/>
       <c r="F103" s="9"/>
-      <c r="G103" s="9"/>
-      <c r="H103" s="9"/>
-      <c r="I103" s="44"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G103" s="44"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="32"/>
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
       <c r="D104" s="7"/>
       <c r="E104" s="9"/>
       <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
-      <c r="H104" s="9"/>
-      <c r="I104" s="44"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G104" s="44"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="32"/>
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
       <c r="D105" s="7"/>
       <c r="E105" s="9"/>
       <c r="F105" s="9"/>
-      <c r="G105" s="9"/>
-      <c r="H105" s="9"/>
-      <c r="I105" s="44"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G105" s="44"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="32"/>
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
       <c r="D106" s="7"/>
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
-      <c r="G106" s="9"/>
-      <c r="H106" s="9"/>
-      <c r="I106" s="44"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G106" s="44"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="32"/>
       <c r="B107" s="10"/>
       <c r="C107" s="10"/>
       <c r="D107" s="7"/>
       <c r="E107" s="9"/>
       <c r="F107" s="9"/>
-      <c r="G107" s="9"/>
-      <c r="H107" s="9"/>
-      <c r="I107" s="44"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G107" s="44"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="32"/>
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
       <c r="D108" s="7"/>
       <c r="E108" s="9"/>
       <c r="F108" s="9"/>
-      <c r="G108" s="9"/>
-      <c r="H108" s="9"/>
-      <c r="I108" s="44"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G108" s="44"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="32"/>
       <c r="B109" s="10"/>
       <c r="C109" s="10"/>
       <c r="D109" s="7"/>
       <c r="E109" s="9"/>
       <c r="F109" s="9"/>
-      <c r="G109" s="9"/>
-      <c r="H109" s="9"/>
-      <c r="I109" s="44"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G109" s="44"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="32"/>
       <c r="B110" s="10"/>
       <c r="C110" s="10"/>
       <c r="D110" s="7"/>
       <c r="E110" s="9"/>
       <c r="F110" s="9"/>
-      <c r="G110" s="9"/>
-      <c r="H110" s="9"/>
-      <c r="I110" s="44"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G110" s="44"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="32"/>
       <c r="B111" s="10"/>
       <c r="C111" s="10"/>
       <c r="D111" s="7"/>
       <c r="E111" s="9"/>
       <c r="F111" s="9"/>
-      <c r="G111" s="9"/>
-      <c r="H111" s="9"/>
-      <c r="I111" s="44"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G111" s="44"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="32"/>
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
       <c r="D112" s="7"/>
       <c r="E112" s="9"/>
       <c r="F112" s="9"/>
-      <c r="G112" s="9"/>
-      <c r="H112" s="9"/>
-      <c r="I112" s="44"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G112" s="44"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="32"/>
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
       <c r="D113" s="7"/>
       <c r="E113" s="9"/>
       <c r="F113" s="9"/>
-      <c r="G113" s="9"/>
-      <c r="H113" s="9"/>
-      <c r="I113" s="44"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G113" s="44"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="32"/>
       <c r="B114" s="10"/>
       <c r="C114" s="10"/>
       <c r="D114" s="7"/>
       <c r="E114" s="9"/>
       <c r="F114" s="9"/>
-      <c r="G114" s="9"/>
-      <c r="H114" s="9"/>
-      <c r="I114" s="44"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G114" s="44"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="32"/>
       <c r="B115" s="10"/>
       <c r="C115" s="10"/>
       <c r="D115" s="7"/>
       <c r="E115" s="9"/>
       <c r="F115" s="9"/>
-      <c r="G115" s="9"/>
-      <c r="H115" s="9"/>
-      <c r="I115" s="44"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G115" s="44"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="32"/>
       <c r="B116" s="10"/>
       <c r="C116" s="10"/>
       <c r="D116" s="7"/>
       <c r="E116" s="9"/>
       <c r="F116" s="9"/>
-      <c r="G116" s="9"/>
-      <c r="H116" s="9"/>
-      <c r="I116" s="44"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G116" s="44"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="32"/>
       <c r="B117" s="10"/>
       <c r="C117" s="10"/>
       <c r="D117" s="7"/>
       <c r="E117" s="9"/>
       <c r="F117" s="9"/>
-      <c r="G117" s="9"/>
-      <c r="H117" s="9"/>
-      <c r="I117" s="44"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G117" s="44"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="32"/>
       <c r="B118" s="10"/>
       <c r="C118" s="10"/>
       <c r="D118" s="7"/>
       <c r="E118" s="9"/>
       <c r="F118" s="9"/>
-      <c r="G118" s="9"/>
-      <c r="H118" s="9"/>
-      <c r="I118" s="44"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G118" s="44"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="32"/>
       <c r="B119" s="10"/>
       <c r="C119" s="10"/>
       <c r="D119" s="7"/>
       <c r="E119" s="9"/>
       <c r="F119" s="9"/>
-      <c r="G119" s="9"/>
-      <c r="H119" s="9"/>
-      <c r="I119" s="44"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G119" s="44"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="32"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
       <c r="D120" s="7"/>
       <c r="E120" s="9"/>
       <c r="F120" s="9"/>
-      <c r="G120" s="9"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="44"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G120" s="44"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="32"/>
       <c r="B121" s="10"/>
       <c r="C121" s="10"/>
       <c r="D121" s="7"/>
       <c r="E121" s="9"/>
       <c r="F121" s="9"/>
-      <c r="G121" s="9"/>
-      <c r="H121" s="9"/>
-      <c r="I121" s="44"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G121" s="44"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="32"/>
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
       <c r="D122" s="7"/>
       <c r="E122" s="9"/>
       <c r="F122" s="9"/>
-      <c r="G122" s="9"/>
-      <c r="H122" s="9"/>
-      <c r="I122" s="44"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G122" s="44"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="32"/>
       <c r="B123" s="10"/>
       <c r="C123" s="10"/>
       <c r="D123" s="7"/>
       <c r="E123" s="9"/>
       <c r="F123" s="9"/>
-      <c r="G123" s="9"/>
-      <c r="H123" s="9"/>
-      <c r="I123" s="44"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G123" s="44"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="32"/>
       <c r="B124" s="10"/>
       <c r="C124" s="10"/>
       <c r="D124" s="7"/>
       <c r="E124" s="9"/>
       <c r="F124" s="9"/>
-      <c r="G124" s="9"/>
-      <c r="H124" s="9"/>
-      <c r="I124" s="44"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G124" s="44"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="32"/>
       <c r="B125" s="10"/>
       <c r="C125" s="10"/>
       <c r="D125" s="7"/>
       <c r="E125" s="9"/>
       <c r="F125" s="9"/>
-      <c r="G125" s="9"/>
-      <c r="H125" s="9"/>
-      <c r="I125" s="44"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G125" s="44"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="32"/>
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
       <c r="D126" s="7"/>
       <c r="E126" s="9"/>
       <c r="F126" s="9"/>
-      <c r="G126" s="9"/>
-      <c r="H126" s="9"/>
-      <c r="I126" s="44"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G126" s="44"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="32"/>
       <c r="B127" s="10"/>
       <c r="C127" s="10"/>
       <c r="D127" s="7"/>
       <c r="E127" s="9"/>
       <c r="F127" s="9"/>
-      <c r="G127" s="9"/>
-      <c r="H127" s="9"/>
-      <c r="I127" s="44"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G127" s="44"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="32"/>
       <c r="B128" s="10"/>
       <c r="C128" s="10"/>
       <c r="D128" s="7"/>
       <c r="E128" s="9"/>
       <c r="F128" s="9"/>
-      <c r="G128" s="9"/>
-      <c r="H128" s="9"/>
-      <c r="I128" s="44"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G128" s="44"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="32"/>
       <c r="B129" s="10"/>
       <c r="C129" s="10"/>
       <c r="D129" s="7"/>
       <c r="E129" s="9"/>
       <c r="F129" s="9"/>
-      <c r="G129" s="9"/>
-      <c r="H129" s="9"/>
-      <c r="I129" s="44"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G129" s="44"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="32"/>
       <c r="B130" s="10"/>
       <c r="C130" s="10"/>
       <c r="D130" s="7"/>
       <c r="E130" s="9"/>
       <c r="F130" s="9"/>
-      <c r="G130" s="9"/>
-      <c r="H130" s="9"/>
-      <c r="I130" s="44"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G130" s="44"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="32"/>
       <c r="B131" s="10"/>
       <c r="C131" s="10"/>
       <c r="D131" s="7"/>
       <c r="E131" s="9"/>
       <c r="F131" s="9"/>
-      <c r="G131" s="9"/>
-      <c r="H131" s="9"/>
-      <c r="I131" s="44"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G131" s="44"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="32"/>
       <c r="B132" s="10"/>
       <c r="C132" s="10"/>
       <c r="D132" s="7"/>
       <c r="E132" s="9"/>
       <c r="F132" s="9"/>
-      <c r="G132" s="9"/>
-      <c r="H132" s="9"/>
-      <c r="I132" s="44"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G132" s="44"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="32"/>
       <c r="B133" s="10"/>
       <c r="C133" s="10"/>
       <c r="D133" s="7"/>
       <c r="E133" s="9"/>
       <c r="F133" s="9"/>
-      <c r="G133" s="9"/>
-      <c r="H133" s="9"/>
-      <c r="I133" s="44"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G133" s="44"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="32"/>
       <c r="B134" s="10"/>
       <c r="C134" s="10"/>
       <c r="D134" s="7"/>
       <c r="E134" s="9"/>
       <c r="F134" s="9"/>
-      <c r="G134" s="9"/>
-      <c r="H134" s="9"/>
-      <c r="I134" s="44"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G134" s="44"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="32"/>
       <c r="B135" s="10"/>
       <c r="C135" s="10"/>
       <c r="D135" s="7"/>
       <c r="E135" s="9"/>
       <c r="F135" s="9"/>
-      <c r="G135" s="9"/>
-      <c r="H135" s="9"/>
-      <c r="I135" s="44"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G135" s="44"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="32"/>
       <c r="B136" s="10"/>
       <c r="C136" s="10"/>
       <c r="D136" s="7"/>
       <c r="E136" s="9"/>
       <c r="F136" s="9"/>
-      <c r="G136" s="9"/>
-      <c r="H136" s="9"/>
-      <c r="I136" s="44"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G136" s="44"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="32"/>
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
       <c r="D137" s="7"/>
       <c r="E137" s="9"/>
       <c r="F137" s="9"/>
-      <c r="G137" s="9"/>
-      <c r="H137" s="9"/>
-      <c r="I137" s="44"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G137" s="44"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="32"/>
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
       <c r="D138" s="7"/>
       <c r="E138" s="9"/>
       <c r="F138" s="9"/>
-      <c r="G138" s="9"/>
-      <c r="H138" s="9"/>
-      <c r="I138" s="44"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G138" s="44"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="32"/>
       <c r="B139" s="10"/>
       <c r="C139" s="10"/>
       <c r="D139" s="7"/>
       <c r="E139" s="9"/>
       <c r="F139" s="9"/>
-      <c r="G139" s="9"/>
-      <c r="H139" s="9"/>
-      <c r="I139" s="44"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G139" s="44"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="32"/>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
       <c r="D140" s="7"/>
       <c r="E140" s="9"/>
       <c r="F140" s="9"/>
-      <c r="G140" s="9"/>
-      <c r="H140" s="9"/>
-      <c r="I140" s="44"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G140" s="44"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="32"/>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
       <c r="D141" s="7"/>
       <c r="E141" s="9"/>
       <c r="F141" s="9"/>
-      <c r="G141" s="9"/>
-      <c r="H141" s="9"/>
-      <c r="I141" s="44"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G141" s="44"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="32"/>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
       <c r="D142" s="7"/>
       <c r="E142" s="9"/>
       <c r="F142" s="9"/>
-      <c r="G142" s="9"/>
-      <c r="H142" s="9"/>
-      <c r="I142" s="44"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G142" s="44"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="32"/>
       <c r="B143" s="10"/>
       <c r="C143" s="10"/>
       <c r="D143" s="7"/>
       <c r="E143" s="9"/>
       <c r="F143" s="9"/>
-      <c r="G143" s="9"/>
-      <c r="H143" s="9"/>
-      <c r="I143" s="44"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G143" s="44"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="32"/>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
       <c r="D144" s="7"/>
       <c r="E144" s="9"/>
       <c r="F144" s="9"/>
-      <c r="G144" s="9"/>
-      <c r="H144" s="9"/>
-      <c r="I144" s="44"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G144" s="44"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="32"/>
       <c r="B145" s="10"/>
       <c r="C145" s="10"/>
       <c r="D145" s="7"/>
       <c r="E145" s="9"/>
       <c r="F145" s="9"/>
-      <c r="G145" s="9"/>
-      <c r="H145" s="9"/>
-      <c r="I145" s="44"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G145" s="44"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="32"/>
       <c r="B146" s="10"/>
       <c r="C146" s="10"/>
       <c r="D146" s="7"/>
       <c r="E146" s="9"/>
       <c r="F146" s="9"/>
-      <c r="G146" s="9"/>
-      <c r="H146" s="9"/>
-      <c r="I146" s="44"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G146" s="44"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="32"/>
       <c r="B147" s="10"/>
       <c r="C147" s="10"/>
       <c r="D147" s="7"/>
       <c r="E147" s="9"/>
       <c r="F147" s="9"/>
-      <c r="G147" s="9"/>
-      <c r="H147" s="9"/>
-      <c r="I147" s="44"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G147" s="44"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="32"/>
       <c r="B148" s="10"/>
       <c r="C148" s="10"/>
       <c r="D148" s="7"/>
       <c r="E148" s="9"/>
       <c r="F148" s="9"/>
-      <c r="G148" s="9"/>
-      <c r="H148" s="9"/>
-      <c r="I148" s="44"/>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G148" s="44"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="32"/>
       <c r="B149" s="10"/>
       <c r="C149" s="10"/>
       <c r="D149" s="7"/>
       <c r="E149" s="9"/>
       <c r="F149" s="9"/>
-      <c r="G149" s="9"/>
-      <c r="H149" s="9"/>
-      <c r="I149" s="44"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G149" s="44"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="32"/>
       <c r="B150" s="10"/>
       <c r="C150" s="10"/>
       <c r="D150" s="7"/>
       <c r="E150" s="9"/>
       <c r="F150" s="9"/>
-      <c r="G150" s="9"/>
-      <c r="H150" s="9"/>
-      <c r="I150" s="44"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G150" s="44"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="32"/>
       <c r="B151" s="10"/>
       <c r="C151" s="10"/>
       <c r="D151" s="7"/>
       <c r="E151" s="9"/>
       <c r="F151" s="9"/>
-      <c r="G151" s="9"/>
-      <c r="H151" s="9"/>
-      <c r="I151" s="44"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G151" s="44"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="32"/>
       <c r="B152" s="10"/>
       <c r="C152" s="10"/>
       <c r="D152" s="7"/>
       <c r="E152" s="9"/>
       <c r="F152" s="9"/>
-      <c r="G152" s="9"/>
-      <c r="H152" s="9"/>
-      <c r="I152" s="44"/>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G152" s="44"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="32"/>
       <c r="B153" s="10"/>
       <c r="C153" s="10"/>
       <c r="D153" s="7"/>
       <c r="E153" s="9"/>
       <c r="F153" s="9"/>
-      <c r="G153" s="9"/>
-      <c r="H153" s="9"/>
-      <c r="I153" s="44"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G153" s="44"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="32"/>
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
       <c r="D154" s="7"/>
       <c r="E154" s="9"/>
       <c r="F154" s="9"/>
-      <c r="G154" s="9"/>
-      <c r="H154" s="9"/>
-      <c r="I154" s="44"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G154" s="44"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="32"/>
       <c r="B155" s="10"/>
       <c r="C155" s="10"/>
       <c r="D155" s="7"/>
       <c r="E155" s="9"/>
       <c r="F155" s="9"/>
-      <c r="G155" s="9"/>
-      <c r="H155" s="9"/>
-      <c r="I155" s="44"/>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G155" s="44"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="32"/>
       <c r="B156" s="10"/>
       <c r="C156" s="10"/>
       <c r="D156" s="7"/>
       <c r="E156" s="9"/>
       <c r="F156" s="9"/>
-      <c r="G156" s="9"/>
-      <c r="H156" s="9"/>
-      <c r="I156" s="44"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G156" s="44"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="32"/>
       <c r="B157" s="10"/>
       <c r="C157" s="10"/>
       <c r="D157" s="7"/>
       <c r="E157" s="9"/>
       <c r="F157" s="9"/>
-      <c r="G157" s="9"/>
-      <c r="H157" s="9"/>
-      <c r="I157" s="44"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G157" s="44"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="32"/>
       <c r="B158" s="10"/>
       <c r="C158" s="10"/>
       <c r="D158" s="7"/>
       <c r="E158" s="9"/>
       <c r="F158" s="9"/>
-      <c r="G158" s="9"/>
-      <c r="H158" s="9"/>
-      <c r="I158" s="44"/>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G158" s="44"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="32"/>
       <c r="B159" s="10"/>
       <c r="C159" s="10"/>
       <c r="D159" s="7"/>
       <c r="E159" s="9"/>
       <c r="F159" s="9"/>
-      <c r="G159" s="9"/>
-      <c r="H159" s="9"/>
-      <c r="I159" s="44"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G159" s="44"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="32"/>
       <c r="B160" s="10"/>
       <c r="C160" s="10"/>
       <c r="D160" s="7"/>
       <c r="E160" s="9"/>
       <c r="F160" s="9"/>
-      <c r="G160" s="9"/>
-      <c r="H160" s="9"/>
-      <c r="I160" s="44"/>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G160" s="44"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="32"/>
       <c r="B161" s="10"/>
       <c r="C161" s="10"/>
       <c r="D161" s="7"/>
       <c r="E161" s="9"/>
       <c r="F161" s="9"/>
-      <c r="G161" s="9"/>
-      <c r="H161" s="9"/>
-      <c r="I161" s="44"/>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G161" s="44"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="32"/>
       <c r="B162" s="10"/>
       <c r="C162" s="10"/>
       <c r="D162" s="7"/>
       <c r="E162" s="9"/>
       <c r="F162" s="9"/>
-      <c r="G162" s="9"/>
-      <c r="H162" s="9"/>
-      <c r="I162" s="44"/>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G162" s="44"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="32"/>
       <c r="B163" s="10"/>
       <c r="C163" s="10"/>
       <c r="D163" s="7"/>
       <c r="E163" s="9"/>
       <c r="F163" s="9"/>
-      <c r="G163" s="9"/>
-      <c r="H163" s="9"/>
-      <c r="I163" s="44"/>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G163" s="44"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="32"/>
       <c r="B164" s="10"/>
       <c r="C164" s="10"/>
       <c r="D164" s="7"/>
       <c r="E164" s="9"/>
       <c r="F164" s="9"/>
-      <c r="G164" s="9"/>
-      <c r="H164" s="9"/>
-      <c r="I164" s="44"/>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G164" s="44"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="32"/>
       <c r="B165" s="10"/>
       <c r="C165" s="10"/>
       <c r="D165" s="7"/>
       <c r="E165" s="9"/>
       <c r="F165" s="9"/>
-      <c r="G165" s="9"/>
-      <c r="H165" s="9"/>
-      <c r="I165" s="44"/>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G165" s="44"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="32"/>
       <c r="B166" s="10"/>
       <c r="C166" s="10"/>
       <c r="D166" s="7"/>
       <c r="E166" s="9"/>
       <c r="F166" s="9"/>
-      <c r="G166" s="9"/>
-      <c r="H166" s="9"/>
-      <c r="I166" s="44"/>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G166" s="44"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="32"/>
       <c r="B167" s="10"/>
       <c r="C167" s="10"/>
       <c r="D167" s="7"/>
       <c r="E167" s="9"/>
       <c r="F167" s="9"/>
-      <c r="G167" s="9"/>
-      <c r="H167" s="9"/>
-      <c r="I167" s="44"/>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G167" s="44"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="32"/>
       <c r="B168" s="10"/>
       <c r="C168" s="10"/>
       <c r="D168" s="7"/>
       <c r="E168" s="9"/>
       <c r="F168" s="9"/>
-      <c r="G168" s="9"/>
-      <c r="H168" s="9"/>
-      <c r="I168" s="44"/>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G168" s="44"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="32"/>
       <c r="B169" s="10"/>
       <c r="C169" s="10"/>
       <c r="D169" s="7"/>
       <c r="E169" s="9"/>
       <c r="F169" s="9"/>
-      <c r="G169" s="9"/>
-      <c r="H169" s="9"/>
-      <c r="I169" s="44"/>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G169" s="44"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="32"/>
       <c r="B170" s="10"/>
       <c r="C170" s="10"/>
       <c r="D170" s="7"/>
       <c r="E170" s="9"/>
       <c r="F170" s="9"/>
-      <c r="G170" s="9"/>
-      <c r="H170" s="9"/>
-      <c r="I170" s="44"/>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G170" s="44"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="32"/>
       <c r="B171" s="10"/>
       <c r="C171" s="10"/>
       <c r="D171" s="7"/>
       <c r="E171" s="9"/>
       <c r="F171" s="9"/>
-      <c r="G171" s="9"/>
-      <c r="H171" s="9"/>
-      <c r="I171" s="44"/>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G171" s="44"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="32"/>
       <c r="B172" s="10"/>
       <c r="C172" s="10"/>
       <c r="D172" s="7"/>
       <c r="E172" s="9"/>
       <c r="F172" s="9"/>
-      <c r="G172" s="9"/>
-      <c r="H172" s="9"/>
-      <c r="I172" s="44"/>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G172" s="44"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="32"/>
       <c r="B173" s="10"/>
       <c r="C173" s="10"/>
       <c r="D173" s="7"/>
       <c r="E173" s="9"/>
       <c r="F173" s="9"/>
-      <c r="G173" s="9"/>
-      <c r="H173" s="9"/>
-      <c r="I173" s="44"/>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G173" s="44"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="32"/>
       <c r="B174" s="10"/>
       <c r="C174" s="10"/>
       <c r="D174" s="7"/>
       <c r="E174" s="9"/>
       <c r="F174" s="9"/>
-      <c r="G174" s="9"/>
-      <c r="H174" s="9"/>
-      <c r="I174" s="44"/>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G174" s="44"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="32"/>
       <c r="B175" s="10"/>
       <c r="C175" s="10"/>
       <c r="D175" s="7"/>
       <c r="E175" s="9"/>
       <c r="F175" s="9"/>
-      <c r="G175" s="9"/>
-      <c r="H175" s="9"/>
-      <c r="I175" s="44"/>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G175" s="44"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="32"/>
       <c r="B176" s="10"/>
       <c r="C176" s="10"/>
       <c r="D176" s="7"/>
       <c r="E176" s="9"/>
       <c r="F176" s="9"/>
-      <c r="G176" s="9"/>
-      <c r="H176" s="9"/>
-      <c r="I176" s="44"/>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G176" s="44"/>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="32"/>
       <c r="B177" s="10"/>
       <c r="C177" s="10"/>
       <c r="D177" s="7"/>
       <c r="E177" s="9"/>
       <c r="F177" s="9"/>
-      <c r="G177" s="9"/>
-      <c r="H177" s="9"/>
-      <c r="I177" s="44"/>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G177" s="44"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="32"/>
       <c r="B178" s="10"/>
       <c r="C178" s="10"/>
       <c r="D178" s="7"/>
       <c r="E178" s="9"/>
       <c r="F178" s="9"/>
-      <c r="G178" s="9"/>
-      <c r="H178" s="9"/>
-      <c r="I178" s="44"/>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G178" s="44"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="32"/>
       <c r="B179" s="10"/>
       <c r="C179" s="10"/>
       <c r="D179" s="7"/>
       <c r="E179" s="9"/>
       <c r="F179" s="9"/>
-      <c r="G179" s="9"/>
-      <c r="H179" s="9"/>
-      <c r="I179" s="44"/>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G179" s="44"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="32"/>
       <c r="B180" s="10"/>
       <c r="C180" s="10"/>
       <c r="D180" s="7"/>
       <c r="E180" s="9"/>
       <c r="F180" s="9"/>
-      <c r="G180" s="9"/>
-      <c r="H180" s="9"/>
-      <c r="I180" s="44"/>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G180" s="44"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="32"/>
       <c r="B181" s="10"/>
       <c r="C181" s="10"/>
       <c r="D181" s="7"/>
       <c r="E181" s="9"/>
       <c r="F181" s="9"/>
-      <c r="G181" s="9"/>
-      <c r="H181" s="9"/>
-      <c r="I181" s="44"/>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G181" s="44"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="32"/>
       <c r="B182" s="10"/>
       <c r="C182" s="10"/>
       <c r="D182" s="7"/>
       <c r="E182" s="9"/>
       <c r="F182" s="9"/>
-      <c r="G182" s="9"/>
-      <c r="H182" s="9"/>
-      <c r="I182" s="44"/>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G182" s="44"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="32"/>
       <c r="B183" s="10"/>
       <c r="C183" s="10"/>
       <c r="D183" s="7"/>
       <c r="E183" s="9"/>
       <c r="F183" s="9"/>
-      <c r="G183" s="9"/>
-      <c r="H183" s="9"/>
-      <c r="I183" s="44"/>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G183" s="44"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="32"/>
       <c r="B184" s="10"/>
       <c r="C184" s="10"/>
       <c r="D184" s="7"/>
       <c r="E184" s="9"/>
       <c r="F184" s="9"/>
-      <c r="G184" s="9"/>
-      <c r="H184" s="9"/>
-      <c r="I184" s="44"/>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G184" s="44"/>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="32"/>
       <c r="B185" s="10"/>
       <c r="C185" s="10"/>
       <c r="D185" s="7"/>
       <c r="E185" s="9"/>
       <c r="F185" s="9"/>
-      <c r="G185" s="9"/>
-      <c r="H185" s="9"/>
-      <c r="I185" s="44"/>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G185" s="44"/>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="32"/>
       <c r="B186" s="10"/>
       <c r="C186" s="10"/>
       <c r="D186" s="7"/>
       <c r="E186" s="9"/>
       <c r="F186" s="9"/>
-      <c r="G186" s="9"/>
-      <c r="H186" s="9"/>
-      <c r="I186" s="44"/>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G186" s="44"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="32"/>
       <c r="B187" s="10"/>
       <c r="C187" s="10"/>
       <c r="D187" s="7"/>
       <c r="E187" s="9"/>
       <c r="F187" s="9"/>
-      <c r="G187" s="9"/>
-      <c r="H187" s="9"/>
-      <c r="I187" s="44"/>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G187" s="44"/>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="32"/>
       <c r="B188" s="10"/>
       <c r="C188" s="10"/>
       <c r="D188" s="7"/>
       <c r="E188" s="9"/>
       <c r="F188" s="9"/>
-      <c r="G188" s="9"/>
-      <c r="H188" s="9"/>
-      <c r="I188" s="44"/>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G188" s="44"/>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="32"/>
       <c r="B189" s="10"/>
       <c r="C189" s="10"/>
       <c r="D189" s="7"/>
       <c r="E189" s="9"/>
       <c r="F189" s="9"/>
-      <c r="G189" s="9"/>
-      <c r="H189" s="9"/>
-      <c r="I189" s="44"/>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G189" s="44"/>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="32"/>
       <c r="B190" s="10"/>
       <c r="C190" s="10"/>
       <c r="D190" s="7"/>
       <c r="E190" s="9"/>
       <c r="F190" s="9"/>
-      <c r="G190" s="9"/>
-      <c r="H190" s="9"/>
-      <c r="I190" s="44"/>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G190" s="44"/>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="32"/>
       <c r="B191" s="10"/>
       <c r="C191" s="10"/>
       <c r="D191" s="7"/>
       <c r="E191" s="9"/>
       <c r="F191" s="9"/>
-      <c r="G191" s="9"/>
-      <c r="H191" s="9"/>
-      <c r="I191" s="44"/>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G191" s="44"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="32"/>
       <c r="B192" s="10"/>
       <c r="C192" s="10"/>
       <c r="D192" s="7"/>
       <c r="E192" s="9"/>
       <c r="F192" s="9"/>
-      <c r="G192" s="9"/>
-      <c r="H192" s="9"/>
-      <c r="I192" s="44"/>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G192" s="44"/>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="32"/>
       <c r="B193" s="10"/>
       <c r="C193" s="10"/>
       <c r="D193" s="7"/>
       <c r="E193" s="9"/>
       <c r="F193" s="9"/>
-      <c r="G193" s="9"/>
-      <c r="H193" s="9"/>
-      <c r="I193" s="44"/>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G193" s="44"/>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="32"/>
       <c r="B194" s="10"/>
       <c r="C194" s="10"/>
       <c r="D194" s="7"/>
       <c r="E194" s="9"/>
       <c r="F194" s="9"/>
-      <c r="G194" s="9"/>
-      <c r="H194" s="9"/>
-      <c r="I194" s="44"/>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G194" s="44"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="32"/>
       <c r="B195" s="10"/>
       <c r="C195" s="10"/>
       <c r="D195" s="7"/>
       <c r="E195" s="9"/>
       <c r="F195" s="9"/>
-      <c r="G195" s="9"/>
-      <c r="H195" s="9"/>
-      <c r="I195" s="44"/>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G195" s="44"/>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="32"/>
       <c r="B196" s="10"/>
       <c r="C196" s="10"/>
       <c r="D196" s="7"/>
       <c r="E196" s="9"/>
       <c r="F196" s="9"/>
-      <c r="G196" s="9"/>
-      <c r="H196" s="9"/>
-      <c r="I196" s="44"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G196" s="44"/>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="32"/>
       <c r="B197" s="10"/>
       <c r="C197" s="10"/>
       <c r="D197" s="7"/>
       <c r="E197" s="9"/>
       <c r="F197" s="9"/>
-      <c r="G197" s="9"/>
-      <c r="H197" s="9"/>
-      <c r="I197" s="44"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G197" s="44"/>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="32"/>
       <c r="B198" s="10"/>
       <c r="C198" s="10"/>
       <c r="D198" s="7"/>
       <c r="E198" s="9"/>
       <c r="F198" s="9"/>
-      <c r="G198" s="9"/>
-      <c r="H198" s="9"/>
-      <c r="I198" s="44"/>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G198" s="44"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="32"/>
       <c r="B199" s="10"/>
       <c r="C199" s="10"/>
       <c r="D199" s="7"/>
       <c r="E199" s="9"/>
       <c r="F199" s="9"/>
-      <c r="G199" s="9"/>
-      <c r="H199" s="9"/>
-      <c r="I199" s="44"/>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G199" s="44"/>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="32"/>
       <c r="B200" s="10"/>
       <c r="C200" s="10"/>
       <c r="D200" s="7"/>
       <c r="E200" s="9"/>
       <c r="F200" s="9"/>
-      <c r="G200" s="9"/>
-      <c r="H200" s="9"/>
-      <c r="I200" s="44"/>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G200" s="44"/>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="33"/>
       <c r="B201" s="11"/>
       <c r="C201" s="11"/>
       <c r="D201" s="12"/>
       <c r="E201" s="13"/>
       <c r="F201" s="13"/>
-      <c r="G201" s="13"/>
-      <c r="H201" s="13"/>
-      <c r="I201" s="46"/>
+      <c r="G201" s="46"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Implement Create global credential Assets
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Assets.xlsx
+++ b/Workbooks/EN/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F5B001-C704-4B51-9C77-C3D9CE2EC01B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5337B23A-2DBB-44BF-9322-29A5D44C023F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>
@@ -406,29 +406,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="59">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1731,6 +1708,29 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
@@ -1820,31 +1820,31 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:I201" headerRowDxfId="58" dataDxfId="56" totalsRowDxfId="54" headerRowBorderDxfId="57" tableBorderDxfId="55">
   <autoFilter ref="A1:I201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Folder ID" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Name" totalsRowFunction="count" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="Asset ID" dataDxfId="52"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Asset Name" totalsRowLabel="Total" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{8E6D9239-8D17-4851-B81E-AA3B7A84B18A}" name="Scope" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{57694A87-E20F-4EA5-8070-3065D32AB335}" name="Robot ID or User ID" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{E62E1B92-1422-4B09-9336-6FC76D703F22}" name="Robot Name or User's Username" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Value" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Folder ID" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Name" totalsRowFunction="count" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="Asset ID" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Asset Name" totalsRowLabel="Total" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{8E6D9239-8D17-4851-B81E-AA3B7A84B18A}" name="Scope" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{57694A87-E20F-4EA5-8070-3065D32AB335}" name="Robot ID or User ID" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{E62E1B92-1422-4B09-9336-6FC76D703F22}" name="Robot Name or User's Username" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Value" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9BB38C27-A0FF-4D4F-AD77-24125AC0FC70}" name="Table148" displayName="Table148" ref="A1:G201" headerRowDxfId="45" dataDxfId="43" totalsRowDxfId="41" headerRowBorderDxfId="44" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9BB38C27-A0FF-4D4F-AD77-24125AC0FC70}" name="Table148" displayName="Table148" ref="A1:G201" headerRowDxfId="44" dataDxfId="42" totalsRowDxfId="40" headerRowBorderDxfId="43" tableBorderDxfId="41">
   <autoFilter ref="A1:G201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="7">
-    <tableColumn id="6" xr3:uid="{485E597C-A24C-40C0-A3EE-E03068634948}" name="Folder ID" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{B6D8F5D0-41CD-4EF8-84D7-03F38C71AB1B}" name="Folder Name" totalsRowFunction="count" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{7208AC74-66FB-4CA6-B9B5-7263FD360340}" name="Credential Asset ID" dataDxfId="38"/>
-    <tableColumn id="1" xr3:uid="{003DAFDE-C24E-41F7-82CA-B0B481F221E2}" name="Credential Asset Name" totalsRowLabel="Total" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{E44775CD-BBCF-4B36-BAE6-DECF89D643E9}" name="Scope" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{DF92207D-0652-4129-89C3-EB38552DB3A7}" name="Username" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{FBA4015B-2D60-460E-9719-EA2C2B95F766}" name="Password" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{485E597C-A24C-40C0-A3EE-E03068634948}" name="Folder ID" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{B6D8F5D0-41CD-4EF8-84D7-03F38C71AB1B}" name="Folder Name" totalsRowFunction="count" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{7208AC74-66FB-4CA6-B9B5-7263FD360340}" name="Credential Asset ID" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{003DAFDE-C24E-41F7-82CA-B0B481F221E2}" name="Credential Asset Name" totalsRowLabel="Total" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{E44775CD-BBCF-4B36-BAE6-DECF89D643E9}" name="Scope" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{DF92207D-0652-4129-89C3-EB38552DB3A7}" name="Username" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{FBA4015B-2D60-460E-9719-EA2C2B95F766}" name="Password" dataDxfId="33" totalsRowDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1854,14 +1854,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H200" totalsRowShown="0">
   <autoFilter ref="A1:H200" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Name" dataDxfId="32"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Asset Name" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{5D69369A-615B-44A7-A44B-274F733D8D7A}" name="Scope" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{FFE08965-A480-4665-AE70-AAA734F3AA96}" name="Robot Name or User's Username" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Asset ID" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Name" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Asset Name" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{5D69369A-615B-44A7-A44B-274F733D8D7A}" name="Scope" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{FFE08965-A480-4665-AE70-AAA734F3AA96}" name="Robot Name or User's Username" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Asset ID" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1871,14 +1871,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AFA36666-423E-4267-B808-DBFD2255CE69}" name="Table16" displayName="Table16" ref="A1:H201" totalsRowShown="0">
   <autoFilter ref="A1:H201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{45AEE497-3A06-46BE-9F75-8739763D4D01}" name="Folder Name" dataDxfId="24"/>
-    <tableColumn id="1" xr3:uid="{9A783E95-B160-494B-86CA-9B17E7B7BA4E}" name="Asset Name" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{30ADF841-3736-4806-AB18-7E5935073536}" name="Scope" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{41C196FB-7963-49FF-96A8-E1B917ABEA29}" name="Robot Name or User's Username" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{003CF074-AEF0-4160-B2A0-AA78FDEF0550}" name="Username" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{B1103FA1-C444-4B4C-B2DE-2AF1F43EE2F7}" name="Password" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{969717FC-5790-4B75-A1B0-2997BE43FE33}" name="Asset ID" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{6C3F9F68-0351-4140-9C48-3AD60D9434AF}" name="Result" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{45AEE497-3A06-46BE-9F75-8739763D4D01}" name="Folder Name" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{9A783E95-B160-494B-86CA-9B17E7B7BA4E}" name="Asset Name" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{30ADF841-3736-4806-AB18-7E5935073536}" name="Scope" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{41C196FB-7963-49FF-96A8-E1B917ABEA29}" name="Robot Name or User's Username" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{003CF074-AEF0-4160-B2A0-AA78FDEF0550}" name="Username" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{B1103FA1-C444-4B4C-B2DE-2AF1F43EE2F7}" name="Password" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{969717FC-5790-4B75-A1B0-2997BE43FE33}" name="Asset ID" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{6C3F9F68-0351-4140-9C48-3AD60D9434AF}" name="Result" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1888,11 +1888,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD40330C-E043-47F5-9A1D-98C4F5DCAE20}" name="Table15" displayName="Table15" ref="A1:E201" totalsRowShown="0">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Name" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Asset ID" dataDxfId="15"/>
-    <tableColumn id="1" xr3:uid="{D002318D-F09E-4941-86F7-CB540B53CA38}" name="Asset Name" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="Value" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Name" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Asset ID" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{D002318D-F09E-4941-86F7-CB540B53CA38}" name="Asset Name" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="Value" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1902,12 +1902,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{343143A2-A745-4DDD-B0DF-0DE2B324A492}" name="Table157" displayName="Table157" ref="A1:F201" totalsRowShown="0">
   <autoFilter ref="A1:F201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="7" xr3:uid="{B324D0A3-E152-4308-B124-7203B73A1BBD}" name="Folder Name" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{2934B7C6-CBD1-40B0-AAC0-BB8AE8E4AE77}" name="Asset ID" dataDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{672D4252-ECDD-4E80-B35E-6A3063360C37}" name="Asset Name" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{4D4E5EE5-4B2B-487A-B22A-AB3842F3C4E6}" name="Username" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{C7C983FA-5C35-471C-8158-BCB2BC1DC74B}" name="Password" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{67DE61C4-5FA9-48B6-AC2A-1392897C0EF9}" name="Result" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{B324D0A3-E152-4308-B124-7203B73A1BBD}" name="Folder Name" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{2934B7C6-CBD1-40B0-AAC0-BB8AE8E4AE77}" name="Asset ID" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{672D4252-ECDD-4E80-B35E-6A3063360C37}" name="Asset Name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{4D4E5EE5-4B2B-487A-B22A-AB3842F3C4E6}" name="Username" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C7C983FA-5C35-471C-8158-BCB2BC1DC74B}" name="Password" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{67DE61C4-5FA9-48B6-AC2A-1392897C0EF9}" name="Result" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1917,11 +1917,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:E201" totalsRowShown="0">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{F24CA0C2-24D3-45F7-8C50-E3B9F93102BC}" name="Folder ID" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Folder Name" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{F81D79E9-4E70-40F0-99EC-DB07CB8A2FD8}" name="Asset ID" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Asset Name" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{F24CA0C2-24D3-45F7-8C50-E3B9F93102BC}" name="Folder ID" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Folder Name" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{F81D79E9-4E70-40F0-99EC-DB07CB8A2FD8}" name="Asset ID" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Asset Name" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2192,7 +2192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
   <dimension ref="A1:I201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8383,7 +8383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56493D34-EA23-4634-A655-5148B0AC19AA}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -10424,9 +10424,12 @@
       <c r="H201" s="6"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Asset ID" error="Asset ID must be an integer greater than 0." sqref="E202:E1048576 G2:G201" xr:uid="{FEC40328-5044-44A3-ACBA-40E7875F6931}">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{F108FDD9-F5CB-43EB-B9FE-A4BDF55B9B1E}">
+      <formula1>"Global,Robot,User"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactor migration of Assets from Classic to Modern Folder
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Assets.xlsx
+++ b/Workbooks/EN/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5337B23A-2DBB-44BF-9322-29A5D44C023F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CE87E4-6F2A-4025-9476-88CAEF1A78D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>
@@ -2192,7 +2192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
   <dimension ref="A1:I201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8383,7 +8383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56493D34-EA23-4634-A655-5148B0AC19AA}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implement migration of Assets per Robot from Classic to Modern Folders
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Assets.xlsx
+++ b/Workbooks/EN/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CE87E4-6F2A-4025-9476-88CAEF1A78D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732AD741-0224-483A-B9D1-F64B5028E30A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
Implement manipulation of Assets per Robot and Assets per User with default value
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Assets.xlsx
+++ b/Workbooks/EN/Assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DD69E6-5E66-417E-9844-643937C34303}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC31163-66F8-49A5-9F08-1E6BAE5BF3E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>

</xml_diff>